<commit_message>
Close to final draft
</commit_message>
<xml_diff>
--- a/Example/xl.xlsx
+++ b/Example/xl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\At work\Documents\My WIP\pdfa3-documents\minimal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HRIDYANSH GAUTAM\Desktop\NPL repo\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAEE18F-3EE6-4BEC-9308-BAB13D8F382A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAFB7B7-9C1E-4090-9235-BD94696310ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32265" yWindow="1815" windowWidth="17880" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test sheet" sheetId="1" r:id="rId1"/>
@@ -337,15 +337,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -359,18 +359,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>1111</v>
       </c>
     </row>

</xml_diff>